<commit_message>
removed role name for non-identity elements in the AlternativeCourseIdentificationCode common in the extension project.
</commit_message>
<xml_diff>
--- a/EdFiXTranscript/MetaEdOutput/Documentation/DataDictionary/SqlDataDictionary.xlsx
+++ b/EdFiXTranscript/MetaEdOutput/Documentation/DataDictionary/SqlDataDictionary.xlsx
@@ -17118,25 +17118,25 @@
         <v>CourseTranscriptAlternativeCourseIdentificationCode</v>
       </c>
       <c r="C381" t="str">
-        <v>AlternativeAssigningOrganizationIdentificationCode</v>
+        <v>AlternativeCourseIdentificationSystemDescriptorId</v>
       </c>
       <c r="D381" t="str">
-        <v>The organization code or name assigning the Identification Code.</v>
+        <v>A system that is used to identify the organization of subject matter and related learning experiences provided for the instruction of students.</v>
       </c>
       <c r="E381" t="str">
-        <v>[NVARCHAR](60)</v>
+        <v>[INT]</v>
       </c>
       <c r="F381" t="str">
-        <v>NULL</v>
+        <v>NOT NULL</v>
       </c>
       <c r="G381" t="str">
         <v>No</v>
       </c>
       <c r="H381" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="I381" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="382">
@@ -17147,16 +17147,16 @@
         <v>CourseTranscriptAlternativeCourseIdentificationCode</v>
       </c>
       <c r="C382" t="str">
-        <v>AlternativeCourseCatalogURL</v>
+        <v>AlternativeIdentificationCode</v>
       </c>
       <c r="D382" t="str">
-        <v>The URL for the course catalog that defines the course identification code.</v>
+        <v>A unique number or alphanumeric code assigned to a course by a school, school system, state, or other agency or entity. For multi-part course codes, concatenate the parts separated by a "/". For example, consider the following SCED code-    subject = 20 Math    course = 272 Geometry    level = G General    credits = 1.00   course sequence 1 of 1- would be entered as 20/272/G/1.00/1 of 1.</v>
       </c>
       <c r="E382" t="str">
-        <v>[NVARCHAR](255)</v>
+        <v>[NVARCHAR](60)</v>
       </c>
       <c r="F382" t="str">
-        <v>NULL</v>
+        <v>NOT NULL</v>
       </c>
       <c r="G382" t="str">
         <v>No</v>
@@ -17170,31 +17170,31 @@
     </row>
     <row r="383">
       <c r="A383" t="str">
-        <v>edfixtranscript</v>
+        <v>edfi</v>
       </c>
       <c r="B383" t="str">
         <v>CourseTranscriptAlternativeCourseIdentificationCode</v>
       </c>
       <c r="C383" t="str">
-        <v>AlternativeCourseIdentificationSystemDescriptorId</v>
+        <v>AssigningOrganizationIdentificationCode</v>
       </c>
       <c r="D383" t="str">
-        <v>A system that is used to identify the organization of subject matter and related learning experiences provided for the instruction of students.</v>
+        <v>The organization code or name assigning the Identification Code.</v>
       </c>
       <c r="E383" t="str">
-        <v>[INT]</v>
+        <v>[NVARCHAR](60)</v>
       </c>
       <c r="F383" t="str">
-        <v>NOT NULL</v>
+        <v>NULL</v>
       </c>
       <c r="G383" t="str">
         <v>No</v>
       </c>
       <c r="H383" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="I383" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
     </row>
     <row r="384">
@@ -17205,16 +17205,16 @@
         <v>CourseTranscriptAlternativeCourseIdentificationCode</v>
       </c>
       <c r="C384" t="str">
-        <v>AlternativeIdentificationCode</v>
+        <v>AssigningOrganizationIdentificationCode</v>
       </c>
       <c r="D384" t="str">
-        <v>A unique number or alphanumeric code assigned to a course by a school, school system, state, or other agency or entity. For multi-part course codes, concatenate the parts separated by a "/". For example, consider the following SCED code-    subject = 20 Math    course = 272 Geometry    level = G General    credits = 1.00   course sequence 1 of 1- would be entered as 20/272/G/1.00/1 of 1.</v>
+        <v>The organization code or name assigning the Identification Code.</v>
       </c>
       <c r="E384" t="str">
         <v>[NVARCHAR](60)</v>
       </c>
       <c r="F384" t="str">
-        <v>NOT NULL</v>
+        <v>NULL</v>
       </c>
       <c r="G384" t="str">
         <v>No</v>
@@ -17226,7 +17226,7 @@
         <v>No</v>
       </c>
     </row>
-    <row r="385">
+    <row r="385" xml:space="preserve">
       <c r="A385" t="str">
         <v>edfi</v>
       </c>
@@ -17234,30 +17234,34 @@
         <v>CourseTranscriptAlternativeCourseIdentificationCode</v>
       </c>
       <c r="C385" t="str">
-        <v>AssigningOrganizationIdentificationCode</v>
-      </c>
-      <c r="D385" t="str">
-        <v>The organization code or name assigning the Identification Code.</v>
+        <v>CourseAttemptResultDescriptorId</v>
+      </c>
+      <c r="D385" t="str" xml:space="preserve">
+        <v xml:space="preserve">The result from the student's attempt to take the course, for example:_x000d_
+        Pass_x000d_
+        Fail_x000d_
+        Incomplete_x000d_
+        Withdrawn.</v>
       </c>
       <c r="E385" t="str">
-        <v>[NVARCHAR](60)</v>
+        <v>[INT]</v>
       </c>
       <c r="F385" t="str">
-        <v>NULL</v>
+        <v>NOT NULL</v>
       </c>
       <c r="G385" t="str">
         <v>No</v>
       </c>
       <c r="H385" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="I385" t="str">
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="386" xml:space="preserve">
       <c r="A386" t="str">
-        <v>edfi</v>
+        <v>edfixtranscript</v>
       </c>
       <c r="B386" t="str">
         <v>CourseTranscriptAlternativeCourseIdentificationCode</v>
@@ -17288,42 +17292,38 @@
         <v>Yes</v>
       </c>
     </row>
-    <row r="387" xml:space="preserve">
+    <row r="387">
       <c r="A387" t="str">
-        <v>edfixtranscript</v>
+        <v>edfi</v>
       </c>
       <c r="B387" t="str">
         <v>CourseTranscriptAlternativeCourseIdentificationCode</v>
       </c>
       <c r="C387" t="str">
-        <v>CourseAttemptResultDescriptorId</v>
-      </c>
-      <c r="D387" t="str" xml:space="preserve">
-        <v xml:space="preserve">The result from the student's attempt to take the course, for example:_x000d_
-        Pass_x000d_
-        Fail_x000d_
-        Incomplete_x000d_
-        Withdrawn.</v>
+        <v>CourseCatalogURL</v>
+      </c>
+      <c r="D387" t="str">
+        <v>The URL for the course catalog that defines the course identification code.</v>
       </c>
       <c r="E387" t="str">
-        <v>[INT]</v>
+        <v>[NVARCHAR](255)</v>
       </c>
       <c r="F387" t="str">
-        <v>NOT NULL</v>
+        <v>NULL</v>
       </c>
       <c r="G387" t="str">
         <v>No</v>
       </c>
       <c r="H387" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="I387" t="str">
-        <v>Yes</v>
+        <v>No</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="str">
-        <v>edfi</v>
+        <v>edfixtranscript</v>
       </c>
       <c r="B388" t="str">
         <v>CourseTranscriptAlternativeCourseIdentificationCode</v>

</xml_diff>